<commit_message>
Minor changes to Financial History test file, csv version of file
</commit_message>
<xml_diff>
--- a/tests/Test_hist.xlsx
+++ b/tests/Test_hist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Date Start</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sum</t>
   </si>
 </sst>
 </file>
@@ -135,12 +132,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -333,192 +334,178 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>45200</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>45230</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>385</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="1" t="n">
         <v>460</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <f aca="false">SUM(E2:L2)</f>
-        <v>585</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>45231</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>45260</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>760</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="1" t="n">
         <v>460</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <f aca="false">SUM(E3:L3)</f>
-        <v>625</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>45261</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>45291</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>990</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4" s="1" t="n">
         <v>460</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <f aca="false">SUM(E4:L4)</f>
-        <v>770</v>
       </c>
     </row>
   </sheetData>

</xml_diff>